<commit_message>
hw3 and project stuff
</commit_message>
<xml_diff>
--- a/Publication-Targets-2019-04-06.xlsx
+++ b/Publication-Targets-2019-04-06.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mark_\Google Drive\AFIT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Marvin\Documents\AFIT Docs\AFIT Git\AFIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0EF87FC-A0F0-4D0A-99BF-2F4E13E291C6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E971C57-2CE1-406D-A61B-B732FE928A26}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10546" xr2:uid="{6229E5B0-4553-4DF4-8385-F2623EDABEF3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6229E5B0-4553-4DF4-8385-F2623EDABEF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Open" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="141">
   <si>
     <t>Notes</t>
   </si>
@@ -433,6 +433,27 @@
   </si>
   <si>
     <t>ACM Transactions on Data Science (TDS)</t>
+  </si>
+  <si>
+    <t>DSAA 2019 : The 6th IEEE International Conference on Data Science and Advanced Analytics (DSAA 2019)</t>
+  </si>
+  <si>
+    <t>5-Oct-19 - 8-Oct-19</t>
+  </si>
+  <si>
+    <t>Washington, D.C.</t>
+  </si>
+  <si>
+    <t>DSAA 2019</t>
+  </si>
+  <si>
+    <t>IEEE Big Data 2019</t>
+  </si>
+  <si>
+    <t>8-Dec - 11 Dec 19</t>
+  </si>
+  <si>
+    <t>Big Data 2019</t>
   </si>
 </sst>
 </file>
@@ -519,7 +540,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -589,6 +610,12 @@
     </xf>
     <xf numFmtId="15" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -905,28 +932,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E43F6859-F51D-48E3-90B7-DF4B16828AD2}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="23.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="23.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.06640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.46484375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.59765625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.53125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.86328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.9296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.19921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.21875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>92</v>
       </c>
@@ -961,7 +988,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>40</v>
       </c>
@@ -996,7 +1023,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>93</v>
       </c>
@@ -1029,7 +1056,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>107</v>
       </c>
@@ -1056,7 +1083,7 @@
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
     </row>
-    <row r="5" spans="1:11" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -1087,7 +1114,7 @@
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>18</v>
       </c>
@@ -1118,7 +1145,7 @@
       <c r="J6" s="11"/>
       <c r="K6" s="11"/>
     </row>
-    <row r="7" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>97</v>
       </c>
@@ -1145,7 +1172,7 @@
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="1:11" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>57</v>
       </c>
@@ -1178,7 +1205,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>53</v>
       </c>
@@ -1209,7 +1236,7 @@
       <c r="J9" s="11"/>
       <c r="K9" s="11"/>
     </row>
-    <row r="10" spans="1:11" ht="57" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>99</v>
       </c>
@@ -1240,7 +1267,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>111</v>
       </c>
@@ -1269,9 +1296,49 @@
       </c>
       <c r="K11" s="11"/>
     </row>
+    <row r="12" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="I12" s="25">
+        <v>43594</v>
+      </c>
+      <c r="J12" s="25">
+        <v>43671</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="24" t="s">
+        <v>140</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:K2" xr:uid="{EB4E30CE-5727-4F37-BD21-3AE9FF01F3F1}"/>
-  <sortState ref="A2:K10">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K10">
     <sortCondition ref="I2:I10"/>
   </sortState>
   <hyperlinks>
@@ -1285,9 +1352,11 @@
     <hyperlink ref="H10" r:id="rId8" xr:uid="{796F609A-893B-4BE0-AE55-FB7FADD2598B}"/>
     <hyperlink ref="H4" r:id="rId9" xr:uid="{3508F7D2-5959-463F-8E29-3BC7B4210FCD}"/>
     <hyperlink ref="H11" r:id="rId10" xr:uid="{D82768B5-0BAB-4287-A47D-0F54A13F11C5}"/>
+    <hyperlink ref="H12" r:id="rId11" xr:uid="{88C3428D-56D5-41E4-B9D3-AF387BFF23D0}"/>
+    <hyperlink ref="H13" r:id="rId12" xr:uid="{66769FEA-6C35-484F-A356-238B3BCCE6A3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
 
@@ -1299,22 +1368,22 @@
       <selection activeCell="A5" sqref="A5:L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="7.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="33.6640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.73046875" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.73046875" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.73046875" style="16" customWidth="1"/>
-    <col min="5" max="5" width="15.46484375" style="16" customWidth="1"/>
-    <col min="6" max="6" width="34.1328125" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.86328125" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.265625" style="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="10.265625" style="16" customWidth="1"/>
-    <col min="12" max="12" width="11.59765625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.77734375" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.77734375" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.77734375" style="16" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" style="16" customWidth="1"/>
+    <col min="6" max="6" width="34.109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.88671875" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.21875" style="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="10.21875" style="16" customWidth="1"/>
+    <col min="12" max="12" width="11.5546875" style="16" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="7.6640625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>120</v>
       </c>
@@ -1352,7 +1421,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="49.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17"/>
       <c r="B2" s="17" t="s">
         <v>116</v>
@@ -1376,7 +1445,7 @@
       <c r="K2" s="20"/>
       <c r="L2" s="17"/>
     </row>
-    <row r="3" spans="1:12" ht="49.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>119</v>
       </c>
@@ -1404,7 +1473,7 @@
       <c r="K3" s="20"/>
       <c r="L3" s="17"/>
     </row>
-    <row r="4" spans="1:12" ht="57" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="17"/>
       <c r="B4" s="17"/>
       <c r="C4" s="17" t="s">
@@ -1424,7 +1493,7 @@
       <c r="K4" s="17"/>
       <c r="L4" s="17"/>
     </row>
-    <row r="5" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="21" t="s">
         <v>132</v>
       </c>
@@ -1478,22 +1547,22 @@
       <selection activeCell="A14" sqref="A14:XFD85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="23.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="23.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.06640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.46484375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.59765625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.53125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.86328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.9296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.19921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.21875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>92</v>
       </c>
@@ -1528,7 +1597,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>46</v>
       </c>
@@ -1557,7 +1626,7 @@
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>73</v>
       </c>
@@ -1588,7 +1657,7 @@
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
     </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>66</v>
       </c>
@@ -1619,7 +1688,7 @@
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
     </row>
-    <row r="5" spans="1:11" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>50</v>
       </c>
@@ -1648,7 +1717,7 @@
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
     </row>
-    <row r="6" spans="1:11" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>77</v>
       </c>
@@ -1679,7 +1748,7 @@
       </c>
       <c r="K6" s="7"/>
     </row>
-    <row r="7" spans="1:11" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>69</v>
       </c>
@@ -1710,7 +1779,7 @@
       <c r="J7" s="15"/>
       <c r="K7" s="15"/>
     </row>
-    <row r="8" spans="1:11" s="1" customFormat="1" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" s="1" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>13</v>
       </c>
@@ -1741,7 +1810,7 @@
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
     </row>
-    <row r="9" spans="1:11" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>22</v>
       </c>
@@ -1772,7 +1841,7 @@
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
     </row>
-    <row r="10" spans="1:11" s="1" customFormat="1" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" s="1" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>81</v>
       </c>
@@ -1805,7 +1874,7 @@
       </c>
       <c r="K10" s="7"/>
     </row>
-    <row r="11" spans="1:11" s="1" customFormat="1" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" s="1" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>26</v>
       </c>
@@ -1834,7 +1903,7 @@
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
     </row>
-    <row r="12" spans="1:11" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>61</v>
       </c>
@@ -1865,7 +1934,7 @@
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
     </row>
-    <row r="13" spans="1:11" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>29</v>
       </c>

</xml_diff>